<commit_message>
jc: actualizar inicio de proyecto
</commit_message>
<xml_diff>
--- a/src/test/resources/data/excelTest.xlsx
+++ b/src/test/resources/data/excelTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">Exitoso</t>
+  </si>
+  <si>
+    <t>fallido</t>
+  </si>
+  <si>
+    <t>exitoso</t>
   </si>
 </sst>
 </file>
@@ -262,8 +268,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="2.76" collapsed="false" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="8.67" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,7 +289,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>123</v>
@@ -295,7 +301,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>456</v>
@@ -307,7 +313,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>789</v>

</xml_diff>